<commit_message>
Custom names in place of original SKU names
</commit_message>
<xml_diff>
--- a/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
+++ b/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Settings\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F389D10-0AC0-4F9C-884C-F4A0AE3E1110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7444349-E055-4748-8875-B43384F9D84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>SL. No</t>
   </si>
@@ -581,6 +581,9 @@
       </rPr>
       <t xml:space="preserve"> this is the user level settings, By default  this is enabled for everyone                                                                                                    1.Select time zone dropdown</t>
     </r>
+  </si>
+  <si>
+    <t>It gets displayed the Perferences</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,6 +1221,12 @@
       <c r="E7" s="8" t="s">
         <v>52</v>
       </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">

</xml_diff>

<commit_message>
Quickbook and Xero testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
+++ b/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Settings\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE791A07-EF7D-4BB9-B72C-300E03A5CDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7808C808-F65D-48A1-8176-C5AD4375D2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>SL. No</t>
   </si>
@@ -422,9 +422,6 @@
     </r>
   </si>
   <si>
-    <t>1.Once click the Xero integration  and enter the credentials ,will get a Authentiction code ,enter and login                                                                                                               2.In supplier mapping Export as dropdown has Select an option</t>
-  </si>
-  <si>
     <t>It displayed  In the integration settings page, if there are any incomplete settings (unmapped), upon clicking "Save" button we will validate and highlight with red outline those that contains errors.</t>
   </si>
   <si>
@@ -603,6 +600,131 @@
   </si>
   <si>
     <t>2.It gets displayed the Perferences</t>
+  </si>
+  <si>
+    <r>
+      <t>1.Once click the '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Xero integration'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  and enter the credentials ,will get a Authentiction code ,enter and login                                                                                                               2.In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Supplier Mapping : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Export as dropdown as Select an supplier, Chart of Account as Select CoA dropdown and Tax rate as N/A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.                                                                                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.In</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Export settings &amp; data mapping : "Export settings and Data mapping" Cancel and Save                                                                                                                                             </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Once click the 'Quickbooks online'  and enter the credentials ,will get a Authentiction code ,enter and login                                                                                                               2.In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Supplier Mapping : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Export as dropdown as Select an supplier, Category as Select Category dropdown and Tax Code as select tax code and Disconnect button</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.In</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Data mapping : "Outlet and Tracking class" Cancel and Save and Disconnect button                                                                                                                                            </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1067,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1314,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -1212,13 +1334,13 @@
         <v>15</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -1235,13 +1357,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -1264,7 +1386,7 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
         <v>31</v>
@@ -1405,7 +1527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -1416,15 +1538,38 @@
         <v>23</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G15" t="s">
+      <c r="E16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Username companies manual testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
+++ b/Buyer hub/Settings/Manual testcases/Settings Final testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Settings\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7808C808-F65D-48A1-8176-C5AD4375D2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9F024C-85F9-4BF3-8B72-10B540515BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>SL. No</t>
   </si>
@@ -903,10 +903,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,6 +1457,9 @@
       <c r="F11" t="s">
         <v>29</v>
       </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">

</xml_diff>